<commit_message>
feat: enhanced logic and UI for exam scheduling system
</commit_message>
<xml_diff>
--- a/backend/output_timetables/exam_schedule_20251120_to_20251205.xlsx
+++ b/backend/output_timetables/exam_schedule_20251120_to_20251205.xlsx
@@ -8,9 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Exam_Schedule" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Summary" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Department_Summary" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Configuration" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,12 +607,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -663,22 +660,22 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -726,12 +723,12 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -789,12 +786,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -852,22 +849,22 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -915,22 +912,22 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -978,12 +975,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1041,12 +1038,12 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Monday</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1104,22 +1101,22 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Monday</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1167,22 +1164,22 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Monday</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1230,12 +1227,12 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Monday</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1293,12 +1290,12 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1325,12 +1322,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>EC302</t>
+          <t>HS201</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Introduction to VLSI Design</t>
+          <t>Happiness &amp; Wellbeing</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1356,27 +1353,27 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2025-04-26</t>
+          <t>2025-04-28</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1419,22 +1416,22 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1451,12 +1448,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>HS201</t>
+          <t>EC302</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Happiness &amp; Wellbeing</t>
+          <t>Introduction to VLSI Design</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1482,12 +1479,12 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1502,7 +1499,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2025-04-28</t>
+          <t>2025-04-26</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1545,12 +1542,12 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1608,22 +1605,22 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1671,7 +1668,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1681,12 +1678,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1734,7 +1731,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1797,7 +1794,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1860,7 +1857,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1870,12 +1867,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -1923,22 +1920,22 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -1986,351 +1983,977 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
+          <t>2025-11-27</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>2025-05-24</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Holistic Personality Development</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1.0 hours</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>60</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>2024-12-27</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>EC304</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Signals &amp; Systems</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>180</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>5</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>2025-05-25</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>MA261</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Differential Equations</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>120</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>EC264</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Semiconductor Devices</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>120</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>5</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>2025-05-26</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>MA262</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Multivariable Calculus</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>120</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>3</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2025-12-01</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>2025-04-16</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>EC262</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Analog Electronics</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>120</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>5</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2025-12-01</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>CS261</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Operating Systems</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>180</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2025-12-01</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>2025-04-17</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CS262</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Software Design</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>180</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>3</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>2025-04-18</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CS253</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Introduction to AI</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>120</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>3</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>2025-04-29</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CS152</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Data Science with Python</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Lab</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>120</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>3</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2025-12-03</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CS309</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Statistics for CS</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>180</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>5</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2025-12-03</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>CS303</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Computer Networks</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>180</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>5</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2025-12-04</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>HS101</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Environmental Studies</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>120</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>5</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2025-12-04</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>CS463</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Parallel Computing</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>180</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>5</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
           <t>2025-12-05</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="I39" t="inlineStr">
         <is>
           <t>Friday</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CS308</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Compiler Design</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Theory</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>180</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>5</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
         <is>
           <t>Afternoon</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="K40" t="inlineStr">
         <is>
           <t>14:00 - 17:00</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>2025-05-24</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>Scheduled</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Total Exams Scheduled</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Exam Period</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Morning Sessions</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Afternoon Sessions</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Theory Exams</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Lab Exams</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Departments Involved</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>24</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-11-20 to 2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>12</v>
-      </c>
-      <c r="D2" t="n">
-        <v>12</v>
-      </c>
-      <c r="E2" t="n">
-        <v>21</v>
-      </c>
-      <c r="F2" t="n">
-        <v>3</v>
-      </c>
-      <c r="G2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Department</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Number of Exams</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Total Duration (min)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Semesters Involved</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Total Duration (hours)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>CSE</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>12</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1620</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>DSAI</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>7</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ECE</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>840</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="n">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Parameter</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Maximum Exams Per Day</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Session Duration (minutes)</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Include Weekends</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Department Conflict Strictness</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>moderate</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Preference Weight</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Session Balance</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>strict</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Allowed Departments</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>CSE, DSAI, ECE, Mathematics, Physics, Humanities</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Allowed Exam Types</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Theory, Lab</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Additional Rules</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>gapDays, sessionLimit, preferMorning</t>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
         </is>
       </c>
     </row>

</xml_diff>